<commit_message>
AddService & AddCareUnit Tests | Functions XML Documentation
</commit_message>
<xml_diff>
--- a/CarePoint/Testing/Testing.xlsx
+++ b/CarePoint/Testing/Testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp TR" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,10 @@
     <sheet name="AddPrescription TC" sheetId="4" r:id="rId4"/>
     <sheet name="SOS TR" sheetId="5" r:id="rId5"/>
     <sheet name="SOS TC" sheetId="6" r:id="rId6"/>
+    <sheet name="Add Service TR" sheetId="7" r:id="rId7"/>
+    <sheet name="Add Service TC" sheetId="8" r:id="rId8"/>
+    <sheet name="Add CareUnit TR" sheetId="9" r:id="rId9"/>
+    <sheet name="Add CareUnit TC" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="264">
   <si>
     <t>Characteristcs</t>
   </si>
@@ -641,9 +645,6 @@
     <t>abilify 10mg tablet</t>
   </si>
   <si>
-    <t>Warning: please make sure that all drugs you typed in step 3 are correctly spelled.</t>
-  </si>
-  <si>
     <t>Remarks Length</t>
   </si>
   <si>
@@ -696,6 +697,129 @@
   </si>
   <si>
     <t>select at least one option</t>
+  </si>
+  <si>
+    <t>Error: please make sure that all drugs you typed in step 3 are correctly spelled.</t>
+  </si>
+  <si>
+    <t>Test Case 6</t>
+  </si>
+  <si>
+    <t>Test Case 7</t>
+  </si>
+  <si>
+    <t>Test Case 8</t>
+  </si>
+  <si>
+    <t>Test Case 9</t>
+  </si>
+  <si>
+    <t>Test Case 10</t>
+  </si>
+  <si>
+    <t>Name Length</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>CategoryId</t>
+  </si>
+  <si>
+    <t>From 1 to 4</t>
+  </si>
+  <si>
+    <t>A1 B1 C1 D1</t>
+  </si>
+  <si>
+    <t>A2 B2 C2 D2</t>
+  </si>
+  <si>
+    <t>A2 B3 C2 D2</t>
+  </si>
+  <si>
+    <t>Test Case 11</t>
+  </si>
+  <si>
+    <t>Test Case 12</t>
+  </si>
+  <si>
+    <t>Test Case 13</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>NameError</t>
+  </si>
+  <si>
+    <t>CategoryIdError</t>
+  </si>
+  <si>
+    <t>CostError</t>
+  </si>
+  <si>
+    <t>The Name field is required.</t>
+  </si>
+  <si>
+    <t>The Category field is required.</t>
+  </si>
+  <si>
+    <t>The Cost field is required.</t>
+  </si>
+  <si>
+    <t>Cost must be greater than or equal 1</t>
+  </si>
+  <si>
+    <t>Greater than or equal 1</t>
+  </si>
+  <si>
+    <t>Less than 1</t>
+  </si>
+  <si>
+    <t>TypeId</t>
+  </si>
+  <si>
+    <t>AvailableRoomCount</t>
+  </si>
+  <si>
+    <t>Less than 0</t>
+  </si>
+  <si>
+    <t>Greater than or equal 0</t>
+  </si>
+  <si>
+    <t>A1 B1 C1 D1 E1</t>
+  </si>
+  <si>
+    <t>A2 B2 C2 D2 E2</t>
+  </si>
+  <si>
+    <t>A2 B3 C3 D2 E2</t>
+  </si>
+  <si>
+    <t>Test Case 14</t>
+  </si>
+  <si>
+    <t>Test Case 15</t>
+  </si>
+  <si>
+    <t>Test Case 16</t>
+  </si>
+  <si>
+    <t>TypeIdError</t>
+  </si>
+  <si>
+    <t>The Type field is required.</t>
+  </si>
+  <si>
+    <t>AvailableRoomCountError</t>
+  </si>
+  <si>
+    <t>The Available Rooms field is required.</t>
+  </si>
+  <si>
+    <t>Please enter a value greater than or equal to 0.</t>
   </si>
 </sst>
 </file>
@@ -778,7 +902,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1164,13 +1288,274 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1261,6 +1646,72 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1280,6 +1731,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1601,10 +2070,10 @@
       <c r="G1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="36"/>
+      <c r="I1" s="58"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -1625,10 +2094,10 @@
       <c r="G2" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="40"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -1649,10 +2118,10 @@
       <c r="G3" s="24">
         <v>1</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="63" t="s">
         <v>157</v>
       </c>
-      <c r="I3" s="42"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -1673,10 +2142,10 @@
       <c r="G4" s="25">
         <v>2</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="60"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -1697,10 +2166,10 @@
       <c r="G5" s="25">
         <v>3</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="59" t="s">
         <v>159</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="60"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
@@ -1717,10 +2186,10 @@
       <c r="G6" s="26">
         <v>4</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="59" t="s">
         <v>173</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="60"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -1737,10 +2206,10 @@
       <c r="G7" s="25">
         <v>5</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="59" t="s">
         <v>160</v>
       </c>
-      <c r="I7" s="38"/>
+      <c r="I7" s="60"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -2161,12 +2630,141 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="43.85546875" customWidth="1"/>
+    <col min="10" max="10" width="40.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A2:S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2646,10 +3244,10 @@
       <c r="F1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -2667,10 +3265,10 @@
       <c r="F2" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="40"/>
+      <c r="H2" s="62"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -2688,10 +3286,10 @@
       <c r="F3" s="24">
         <v>1</v>
       </c>
-      <c r="G3" s="41" t="s">
-        <v>207</v>
-      </c>
-      <c r="H3" s="42"/>
+      <c r="G3" s="63" t="s">
+        <v>206</v>
+      </c>
+      <c r="H3" s="64"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -2707,10 +3305,10 @@
       <c r="F4" s="25">
         <v>2</v>
       </c>
-      <c r="G4" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="H4" s="38"/>
+      <c r="G4" s="59" t="s">
+        <v>207</v>
+      </c>
+      <c r="H4" s="60"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -2728,10 +3326,10 @@
       <c r="F5" s="25">
         <v>3</v>
       </c>
-      <c r="G5" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="H5" s="38"/>
+      <c r="G5" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="H5" s="60"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -2759,7 +3357,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B8" s="19">
         <v>0</v>
@@ -2870,7 +3468,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>43</v>
@@ -2898,8 +3496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection sqref="A1:P4"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2955,7 +3553,7 @@
         <v>193</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>194</v>
@@ -2963,7 +3561,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>168</v>
+        <v>224</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>195</v>
@@ -2989,7 +3587,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>169</v>
+        <v>225</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>164</v>
@@ -3023,13 +3621,13 @@
       <c r="O3" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>205</v>
+      <c r="P3" s="37" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>170</v>
+        <v>226</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>151</v>
@@ -3110,14 +3708,14 @@
       <c r="E1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="G1" s="36"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="35">
         <v>0</v>
@@ -3128,14 +3726,14 @@
       <c r="E2" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="40"/>
+      <c r="G2" s="62"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B3" s="35">
         <v>0</v>
@@ -3146,10 +3744,10 @@
       <c r="E3" s="24">
         <v>1</v>
       </c>
-      <c r="F3" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="G3" s="42"/>
+      <c r="F3" s="63" t="s">
+        <v>212</v>
+      </c>
+      <c r="G3" s="64"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
@@ -3157,10 +3755,10 @@
       <c r="E4" s="25">
         <v>2</v>
       </c>
-      <c r="F4" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="G4" s="38"/>
+      <c r="F4" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="G4" s="60"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
@@ -3175,7 +3773,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>27</v>
@@ -3186,7 +3784,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7" s="35" t="s">
         <v>30</v>
@@ -3210,8 +3808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3226,31 +3824,31 @@
         <v>70</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>219</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>168</v>
+        <v>227</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>203</v>
@@ -3262,15 +3860,15 @@
         <v>203</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>169</v>
+        <v>228</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -3287,4 +3885,524 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="9" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="67"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="36">
+        <v>0</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="43"/>
+      <c r="F2" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="62"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>247</v>
+      </c>
+      <c r="F3" s="52">
+        <v>1</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3" s="68"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="19">
+        <v>0</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="D4" s="43"/>
+      <c r="F4" s="53">
+        <v>2</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="H4" s="65"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="47">
+        <v>0</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="49"/>
+      <c r="F5" s="55">
+        <v>3</v>
+      </c>
+      <c r="G5" s="69" t="s">
+        <v>235</v>
+      </c>
+      <c r="H5" s="70"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="43"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="43"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G5:H5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="8" max="16" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="67"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="38">
+        <v>0</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="54"/>
+      <c r="F2" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="62"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>247</v>
+      </c>
+      <c r="F3" s="52">
+        <v>1</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" s="68"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="44" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>252</v>
+      </c>
+      <c r="F4" s="52">
+        <v>2</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>254</v>
+      </c>
+      <c r="H4" s="68"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="19">
+        <v>0</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="54"/>
+      <c r="F5" s="52">
+        <v>3</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>255</v>
+      </c>
+      <c r="H5" s="65"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" s="47">
+        <v>0</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="D6" s="57"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="54"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="54"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>